<commit_message>
Fix: Implement bulletproof fill function with title attribute matching for Oracle fields
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -702,7 +702,7 @@
         <v>click</v>
       </c>
       <c r="I9" t="str">
-        <v>Enter Query</v>
+        <v>New</v>
       </c>
       <c r="K9" t="str">
         <v xml:space="preserve">New should be clicked </v>
@@ -714,7 +714,7 @@
         <v>Could not click element</v>
       </c>
       <c r="N9" t="str">
-        <v>Failed to click: Enter Query</v>
+        <v>Failed to click: New</v>
       </c>
       <c r="O9" t="str">
         <v>screenshots/STEP_8.png</v>
@@ -1070,10 +1070,7 @@
         <v>Click</v>
       </c>
       <c r="I25" t="str">
-        <v>Enter Query</v>
-      </c>
-      <c r="J25" t="str">
-        <v>Enter Query</v>
+        <v xml:space="preserve">Enter Query </v>
       </c>
       <c r="K25" t="str">
         <v xml:space="preserve">Enter Query should be clicked </v>

</xml_diff>

<commit_message>
Remove standalone simplified_search.ts - code already merged into assistant.ts
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -742,21 +742,6 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
-      <c r="L10" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M10" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N10" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O10" t="str">
-        <v/>
-      </c>
-      <c r="P10" t="str">
-        <v/>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -780,21 +765,6 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
-      <c r="L11" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M11" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N11" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O11" t="str">
-        <v/>
-      </c>
-      <c r="P11" t="str">
-        <v/>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -818,21 +788,6 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
-      <c r="L12" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M12" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N12" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O12" t="str">
-        <v/>
-      </c>
-      <c r="P12" t="str">
-        <v/>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -856,21 +811,6 @@
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
       </c>
-      <c r="L13" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M13" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N13" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O13" t="str">
-        <v/>
-      </c>
-      <c r="P13" t="str">
-        <v/>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -894,21 +834,6 @@
       <c r="K14" t="str">
         <v xml:space="preserve">Address1 should be filled </v>
       </c>
-      <c r="L14" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M14" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N14" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O14" t="str">
-        <v/>
-      </c>
-      <c r="P14" t="str">
-        <v/>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -932,21 +857,6 @@
       <c r="K15" t="str">
         <v xml:space="preserve">Country should be filled </v>
       </c>
-      <c r="L15" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M15" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N15" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O15" t="str">
-        <v/>
-      </c>
-      <c r="P15" t="str">
-        <v/>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -970,21 +880,6 @@
       <c r="K16" t="str">
         <v xml:space="preserve">Nationality should be filled </v>
       </c>
-      <c r="L16" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M16" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N16" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O16" t="str">
-        <v/>
-      </c>
-      <c r="P16" t="str">
-        <v/>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1008,21 +903,6 @@
       <c r="K17" t="str">
         <v xml:space="preserve">Gender should clicked </v>
       </c>
-      <c r="L17" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M17" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N17" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O17" t="str">
-        <v/>
-      </c>
-      <c r="P17" t="str">
-        <v/>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1046,21 +926,6 @@
       <c r="K18" t="str">
         <v xml:space="preserve">DOB should be entered </v>
       </c>
-      <c r="L18" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M18" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N18" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O18" t="str">
-        <v/>
-      </c>
-      <c r="P18" t="str">
-        <v/>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1084,21 +949,6 @@
       <c r="K19" t="str">
         <v xml:space="preserve">Language should be entered </v>
       </c>
-      <c r="L19" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M19" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N19" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O19" t="str">
-        <v/>
-      </c>
-      <c r="P19" t="str">
-        <v/>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1119,21 +969,6 @@
       <c r="K20" t="str">
         <v xml:space="preserve">Additional should be clicked </v>
       </c>
-      <c r="L20" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M20" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N20" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O20" t="str">
-        <v/>
-      </c>
-      <c r="P20" t="str">
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1157,21 +992,6 @@
       <c r="K21" t="str">
         <v xml:space="preserve">Location should be filled </v>
       </c>
-      <c r="L21" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M21" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N21" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O21" t="str">
-        <v/>
-      </c>
-      <c r="P21" t="str">
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1195,21 +1015,6 @@
       <c r="K22" t="str">
         <v xml:space="preserve">Media should be filled </v>
       </c>
-      <c r="L22" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M22" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N22" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O22" t="str">
-        <v/>
-      </c>
-      <c r="P22" t="str">
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1230,21 +1035,6 @@
       <c r="K23" t="str">
         <v xml:space="preserve">Save should be clicked </v>
       </c>
-      <c r="L23" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M23" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N23" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O23" t="str">
-        <v/>
-      </c>
-      <c r="P23" t="str">
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1265,21 +1055,6 @@
       <c r="K24" t="str">
         <v xml:space="preserve">Accept should be clicked </v>
       </c>
-      <c r="L24" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M24" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N24" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O24" t="str">
-        <v/>
-      </c>
-      <c r="P24" t="str">
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1300,12 +1075,6 @@
       <c r="K25" t="str">
         <v xml:space="preserve">Enter Query should be clicked </v>
       </c>
-      <c r="L25" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M25" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1329,12 +1098,6 @@
       <c r="K26" t="str">
         <v>Customer number should be entered</v>
       </c>
-      <c r="L26" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M26" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1358,12 +1121,6 @@
       <c r="K27" t="str">
         <v>Currency should be entered</v>
       </c>
-      <c r="L27" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M27" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1387,12 +1144,6 @@
       <c r="K28" t="str">
         <v>Account class should be entered</v>
       </c>
-      <c r="L28" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M28" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1413,12 +1164,6 @@
       <c r="K29" t="str">
         <v>Fetch button should be clicked</v>
       </c>
-      <c r="L29" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M29" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1442,12 +1187,6 @@
       <c r="K30" t="str">
         <v>Location should be entered</v>
       </c>
-      <c r="L30" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M30" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1471,12 +1210,6 @@
       <c r="K31" t="str">
         <v>Media should be entered</v>
       </c>
-      <c r="L31" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M31" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1500,12 +1233,6 @@
       <c r="K32" t="str">
         <v xml:space="preserve">Pool code should be entered </v>
       </c>
-      <c r="L32" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M32" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1526,12 +1253,6 @@
       <c r="K33" t="str">
         <v xml:space="preserve">Save and Select accept should be clicked </v>
       </c>
-      <c r="L33" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M33" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1564,12 +1285,6 @@
       <c r="K34" t="str">
         <v>URL should be opened</v>
       </c>
-      <c r="L34" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M34" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1590,12 +1305,6 @@
       <c r="K35" t="str">
         <v>Login should be clicked</v>
       </c>
-      <c r="L35" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M35" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1616,12 +1325,6 @@
       <c r="K36" t="str">
         <v>Men should be clicked</v>
       </c>
-      <c r="L36" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M36" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1642,12 +1345,6 @@
       <c r="K37" t="str">
         <v>Running shoes should be clicked</v>
       </c>
-      <c r="L37" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M37" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1668,12 +1365,6 @@
       <c r="K38" t="str">
         <v xml:space="preserve">COLOR should be clicked </v>
       </c>
-      <c r="L38" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M38" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1694,12 +1385,6 @@
       <c r="K39" t="str">
         <v>Blue should be selected</v>
       </c>
-      <c r="L39" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M39" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1719,12 +1404,6 @@
       </c>
       <c r="K40" t="str">
         <v xml:space="preserve">Best seller product should be clicked </v>
-      </c>
-      <c r="L40" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M40" t="str">
-        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve overlay element visibility detection - be more lenient with hidden CSS properties
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -487,19 +487,19 @@
         <v xml:space="preserve">URL is opened </v>
       </c>
       <c r="L2" t="str">
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="M2" t="str">
-        <v>Cannot read properties of null (reading 'isClosed')</v>
+        <v/>
       </c>
       <c r="N2" t="str">
-        <v>Cannot read properties of null (reading 'isClosed')</v>
+        <v>Opened: https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
       </c>
       <c r="O2" t="str">
-        <v/>
+        <v>screenshots/STEP_1.png</v>
       </c>
       <c r="P2" t="str">
-        <v/>
+        <v>page_sources/STEP_1_source.html</v>
       </c>
     </row>
     <row r="3">
@@ -524,6 +524,12 @@
       <c r="K3" t="str">
         <v>username should be entered</v>
       </c>
+      <c r="L3" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M3" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -547,6 +553,12 @@
       <c r="K4" t="str">
         <v>password should be entered</v>
       </c>
+      <c r="L4" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M4" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -567,6 +579,12 @@
       <c r="K5" t="str">
         <v>Sign in button should be clicked</v>
       </c>
+      <c r="L5" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M5" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -584,6 +602,12 @@
       <c r="I6" t="str">
         <v>Ok</v>
       </c>
+      <c r="L6" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M6" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -613,6 +637,21 @@
       <c r="K7" t="str">
         <v>Fucntion Id should be filled with STDCIF</v>
       </c>
+      <c r="L7" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v>Filled: Function Id</v>
+      </c>
+      <c r="O7" t="str">
+        <v>screenshots/STEP_6.png</v>
+      </c>
+      <c r="P7" t="str">
+        <v>page_sources/STEP_6_source.html</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -633,6 +672,21 @@
       <c r="K8" t="str">
         <v xml:space="preserve">GO button should be clicked </v>
       </c>
+      <c r="L8" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v>Clicked: Go</v>
+      </c>
+      <c r="O8" t="str">
+        <v>screenshots/STEP_7.png</v>
+      </c>
+      <c r="P8" t="str">
+        <v>page_sources/STEP_7_source.html</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -653,6 +707,21 @@
       <c r="K9" t="str">
         <v xml:space="preserve">New should be clicked </v>
       </c>
+      <c r="L9" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M9" t="str">
+        <v>Could not click element</v>
+      </c>
+      <c r="N9" t="str">
+        <v>Failed to click: New</v>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -673,6 +742,21 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
+      <c r="L10" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M10" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N10" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O10" t="str">
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -696,6 +780,21 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
+      <c r="L11" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M11" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N11" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O11" t="str">
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -719,6 +818,21 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
+      <c r="L12" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M12" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N12" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -742,6 +856,21 @@
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
       </c>
+      <c r="L13" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M13" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N13" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O13" t="str">
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -765,6 +894,21 @@
       <c r="K14" t="str">
         <v xml:space="preserve">Address1 should be filled </v>
       </c>
+      <c r="L14" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M14" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N14" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O14" t="str">
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -788,6 +932,21 @@
       <c r="K15" t="str">
         <v xml:space="preserve">Country should be filled </v>
       </c>
+      <c r="L15" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M15" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N15" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -811,6 +970,21 @@
       <c r="K16" t="str">
         <v xml:space="preserve">Nationality should be filled </v>
       </c>
+      <c r="L16" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M16" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N16" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O16" t="str">
+        <v/>
+      </c>
+      <c r="P16" t="str">
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -834,6 +1008,21 @@
       <c r="K17" t="str">
         <v xml:space="preserve">Gender should clicked </v>
       </c>
+      <c r="L17" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M17" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N17" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -857,6 +1046,21 @@
       <c r="K18" t="str">
         <v xml:space="preserve">DOB should be entered </v>
       </c>
+      <c r="L18" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M18" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N18" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -880,6 +1084,21 @@
       <c r="K19" t="str">
         <v xml:space="preserve">Language should be entered </v>
       </c>
+      <c r="L19" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M19" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N19" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -900,6 +1119,21 @@
       <c r="K20" t="str">
         <v xml:space="preserve">Additional should be clicked </v>
       </c>
+      <c r="L20" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M20" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N20" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -923,6 +1157,21 @@
       <c r="K21" t="str">
         <v xml:space="preserve">Location should be filled </v>
       </c>
+      <c r="L21" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M21" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N21" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -946,6 +1195,21 @@
       <c r="K22" t="str">
         <v xml:space="preserve">Media should be filled </v>
       </c>
+      <c r="L22" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M22" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N22" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -966,6 +1230,21 @@
       <c r="K23" t="str">
         <v xml:space="preserve">Save should be clicked </v>
       </c>
+      <c r="L23" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M23" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N23" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -986,6 +1265,21 @@
       <c r="K24" t="str">
         <v xml:space="preserve">Accept should be clicked </v>
       </c>
+      <c r="L24" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M24" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="N24" t="str">
+        <v>No valid page available</v>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1006,6 +1300,12 @@
       <c r="K25" t="str">
         <v xml:space="preserve">Enter Query should be clicked </v>
       </c>
+      <c r="L25" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M25" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1029,6 +1329,12 @@
       <c r="K26" t="str">
         <v>Customer number should be entered</v>
       </c>
+      <c r="L26" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M26" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1052,6 +1358,12 @@
       <c r="K27" t="str">
         <v>Currency should be entered</v>
       </c>
+      <c r="L27" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M27" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1075,6 +1387,12 @@
       <c r="K28" t="str">
         <v>Account class should be entered</v>
       </c>
+      <c r="L28" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M28" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1095,6 +1413,12 @@
       <c r="K29" t="str">
         <v>Fetch button should be clicked</v>
       </c>
+      <c r="L29" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M29" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1118,6 +1442,12 @@
       <c r="K30" t="str">
         <v>Location should be entered</v>
       </c>
+      <c r="L30" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M30" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1141,6 +1471,12 @@
       <c r="K31" t="str">
         <v>Media should be entered</v>
       </c>
+      <c r="L31" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M31" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1164,6 +1500,12 @@
       <c r="K32" t="str">
         <v xml:space="preserve">Pool code should be entered </v>
       </c>
+      <c r="L32" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M32" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1184,6 +1526,12 @@
       <c r="K33" t="str">
         <v xml:space="preserve">Save and Select accept should be clicked </v>
       </c>
+      <c r="L33" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M33" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1216,6 +1564,12 @@
       <c r="K34" t="str">
         <v>URL should be opened</v>
       </c>
+      <c r="L34" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M34" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1236,6 +1590,12 @@
       <c r="K35" t="str">
         <v>Login should be clicked</v>
       </c>
+      <c r="L35" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M35" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1256,6 +1616,12 @@
       <c r="K36" t="str">
         <v>Men should be clicked</v>
       </c>
+      <c r="L36" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M36" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1276,6 +1642,12 @@
       <c r="K37" t="str">
         <v>Running shoes should be clicked</v>
       </c>
+      <c r="L37" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M37" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1296,6 +1668,12 @@
       <c r="K38" t="str">
         <v xml:space="preserve">COLOR should be clicked </v>
       </c>
+      <c r="L38" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M38" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1316,6 +1694,12 @@
       <c r="K39" t="str">
         <v>Blue should be selected</v>
       </c>
+      <c r="L39" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M39" t="str">
+        <v>TO BE EXECUTED = NO</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1335,6 +1719,12 @@
       </c>
       <c r="K40" t="str">
         <v xml:space="preserve">Best seller product should be clicked </v>
+      </c>
+      <c r="L40" t="str">
+        <v>SKIPPED</v>
+      </c>
+      <c r="M40" t="str">
+        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add smart auto-scroll behavior to log steps - scrolls to latest unless user manually scrolling
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -742,21 +742,6 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
-      <c r="L10" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M10" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N10" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O10" t="str">
-        <v/>
-      </c>
-      <c r="P10" t="str">
-        <v/>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -780,21 +765,6 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
-      <c r="L11" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M11" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N11" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O11" t="str">
-        <v/>
-      </c>
-      <c r="P11" t="str">
-        <v/>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -818,21 +788,6 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
-      <c r="L12" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M12" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N12" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O12" t="str">
-        <v/>
-      </c>
-      <c r="P12" t="str">
-        <v/>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -856,21 +811,6 @@
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
       </c>
-      <c r="L13" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M13" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N13" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O13" t="str">
-        <v/>
-      </c>
-      <c r="P13" t="str">
-        <v/>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -894,21 +834,6 @@
       <c r="K14" t="str">
         <v xml:space="preserve">Address1 should be filled </v>
       </c>
-      <c r="L14" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M14" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N14" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O14" t="str">
-        <v/>
-      </c>
-      <c r="P14" t="str">
-        <v/>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -932,21 +857,6 @@
       <c r="K15" t="str">
         <v xml:space="preserve">Country should be filled </v>
       </c>
-      <c r="L15" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M15" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N15" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O15" t="str">
-        <v/>
-      </c>
-      <c r="P15" t="str">
-        <v/>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -970,21 +880,6 @@
       <c r="K16" t="str">
         <v xml:space="preserve">Nationality should be filled </v>
       </c>
-      <c r="L16" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M16" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N16" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O16" t="str">
-        <v/>
-      </c>
-      <c r="P16" t="str">
-        <v/>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -1008,21 +903,6 @@
       <c r="K17" t="str">
         <v xml:space="preserve">Gender should clicked </v>
       </c>
-      <c r="L17" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M17" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N17" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O17" t="str">
-        <v/>
-      </c>
-      <c r="P17" t="str">
-        <v/>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1046,21 +926,6 @@
       <c r="K18" t="str">
         <v xml:space="preserve">DOB should be entered </v>
       </c>
-      <c r="L18" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M18" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N18" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O18" t="str">
-        <v/>
-      </c>
-      <c r="P18" t="str">
-        <v/>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1084,21 +949,6 @@
       <c r="K19" t="str">
         <v xml:space="preserve">Language should be entered </v>
       </c>
-      <c r="L19" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M19" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N19" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O19" t="str">
-        <v/>
-      </c>
-      <c r="P19" t="str">
-        <v/>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1119,21 +969,6 @@
       <c r="K20" t="str">
         <v xml:space="preserve">Additional should be clicked </v>
       </c>
-      <c r="L20" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M20" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N20" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O20" t="str">
-        <v/>
-      </c>
-      <c r="P20" t="str">
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1157,21 +992,6 @@
       <c r="K21" t="str">
         <v xml:space="preserve">Location should be filled </v>
       </c>
-      <c r="L21" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M21" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N21" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O21" t="str">
-        <v/>
-      </c>
-      <c r="P21" t="str">
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1195,21 +1015,6 @@
       <c r="K22" t="str">
         <v xml:space="preserve">Media should be filled </v>
       </c>
-      <c r="L22" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M22" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N22" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O22" t="str">
-        <v/>
-      </c>
-      <c r="P22" t="str">
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1230,21 +1035,6 @@
       <c r="K23" t="str">
         <v xml:space="preserve">Save should be clicked </v>
       </c>
-      <c r="L23" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M23" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N23" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O23" t="str">
-        <v/>
-      </c>
-      <c r="P23" t="str">
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1265,21 +1055,6 @@
       <c r="K24" t="str">
         <v xml:space="preserve">Accept should be clicked </v>
       </c>
-      <c r="L24" t="str">
-        <v>FAIL</v>
-      </c>
-      <c r="M24" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="N24" t="str">
-        <v>No valid page available</v>
-      </c>
-      <c r="O24" t="str">
-        <v/>
-      </c>
-      <c r="P24" t="str">
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1300,12 +1075,6 @@
       <c r="K25" t="str">
         <v xml:space="preserve">Enter Query should be clicked </v>
       </c>
-      <c r="L25" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M25" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1329,12 +1098,6 @@
       <c r="K26" t="str">
         <v>Customer number should be entered</v>
       </c>
-      <c r="L26" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M26" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1358,12 +1121,6 @@
       <c r="K27" t="str">
         <v>Currency should be entered</v>
       </c>
-      <c r="L27" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M27" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1387,12 +1144,6 @@
       <c r="K28" t="str">
         <v>Account class should be entered</v>
       </c>
-      <c r="L28" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M28" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1413,12 +1164,6 @@
       <c r="K29" t="str">
         <v>Fetch button should be clicked</v>
       </c>
-      <c r="L29" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M29" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1442,12 +1187,6 @@
       <c r="K30" t="str">
         <v>Location should be entered</v>
       </c>
-      <c r="L30" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M30" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1471,12 +1210,6 @@
       <c r="K31" t="str">
         <v>Media should be entered</v>
       </c>
-      <c r="L31" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M31" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1500,12 +1233,6 @@
       <c r="K32" t="str">
         <v xml:space="preserve">Pool code should be entered </v>
       </c>
-      <c r="L32" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M32" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1526,12 +1253,6 @@
       <c r="K33" t="str">
         <v xml:space="preserve">Save and Select accept should be clicked </v>
       </c>
-      <c r="L33" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M33" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1564,12 +1285,6 @@
       <c r="K34" t="str">
         <v>URL should be opened</v>
       </c>
-      <c r="L34" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M34" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1590,12 +1305,6 @@
       <c r="K35" t="str">
         <v>Login should be clicked</v>
       </c>
-      <c r="L35" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M35" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1616,12 +1325,6 @@
       <c r="K36" t="str">
         <v>Men should be clicked</v>
       </c>
-      <c r="L36" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M36" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1642,12 +1345,6 @@
       <c r="K37" t="str">
         <v>Running shoes should be clicked</v>
       </c>
-      <c r="L37" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M37" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1668,12 +1365,6 @@
       <c r="K38" t="str">
         <v xml:space="preserve">COLOR should be clicked </v>
       </c>
-      <c r="L38" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M38" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1694,12 +1385,6 @@
       <c r="K39" t="str">
         <v>Blue should be selected</v>
       </c>
-      <c r="L39" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M39" t="str">
-        <v>TO BE EXECUTED = NO</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1719,12 +1404,6 @@
       </c>
       <c r="K40" t="str">
         <v xml:space="preserve">Best seller product should be clicked </v>
-      </c>
-      <c r="L40" t="str">
-        <v>SKIPPED</v>
-      </c>
-      <c r="M40" t="str">
-        <v>TO BE EXECUTED = NO</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Prioritize latest subwindow in BOTH click and fill operations - Check priority window FIRST before main window strategies
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -708,19 +708,19 @@
         <v xml:space="preserve">New should be clicked </v>
       </c>
       <c r="L9" t="str">
-        <v>FAIL</v>
+        <v>PASS</v>
       </c>
       <c r="M9" t="str">
-        <v>Could not click element</v>
+        <v/>
       </c>
       <c r="N9" t="str">
-        <v>Failed to click: New</v>
+        <v>Clicked: New</v>
       </c>
       <c r="O9" t="str">
-        <v/>
+        <v>screenshots/STEP_8.png</v>
       </c>
       <c r="P9" t="str">
-        <v/>
+        <v>page_sources/STEP_8_source.html</v>
       </c>
     </row>
     <row r="10">
@@ -742,6 +742,21 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
+      <c r="L10" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v>Clicked: P</v>
+      </c>
+      <c r="O10" t="str">
+        <v>screenshots/STEP_9.png</v>
+      </c>
+      <c r="P10" t="str">
+        <v>page_sources/STEP_9_source.html</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -765,6 +780,21 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
+      <c r="L11" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v>Filled: Full Name</v>
+      </c>
+      <c r="O11" t="str">
+        <v>screenshots/STEP_10.png</v>
+      </c>
+      <c r="P11" t="str">
+        <v>page_sources/STEP_10_source.html</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -788,6 +818,21 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
+      <c r="L12" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v>Filled: Short Name</v>
+      </c>
+      <c r="O12" t="str">
+        <v>screenshots/STEP_11.png</v>
+      </c>
+      <c r="P12" t="str">
+        <v>page_sources/STEP_11_source.html</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -811,6 +856,21 @@
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
       </c>
+      <c r="L13" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v>Filled: Customer Category</v>
+      </c>
+      <c r="O13" t="str">
+        <v>screenshots/STEP_12.png</v>
+      </c>
+      <c r="P13" t="str">
+        <v>page_sources/STEP_12_source.html</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -834,6 +894,21 @@
       <c r="K14" t="str">
         <v xml:space="preserve">Address1 should be filled </v>
       </c>
+      <c r="L14" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v>Filled: Address 1</v>
+      </c>
+      <c r="O14" t="str">
+        <v>screenshots/STEP_13.png</v>
+      </c>
+      <c r="P14" t="str">
+        <v>page_sources/STEP_13_source.html</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -857,6 +932,21 @@
       <c r="K15" t="str">
         <v xml:space="preserve">Country should be filled </v>
       </c>
+      <c r="L15" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <v>Filled: Country</v>
+      </c>
+      <c r="O15" t="str">
+        <v>screenshots/STEP_14.png</v>
+      </c>
+      <c r="P15" t="str">
+        <v>page_sources/STEP_14_source.html</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -880,6 +970,21 @@
       <c r="K16" t="str">
         <v xml:space="preserve">Nationality should be filled </v>
       </c>
+      <c r="L16" t="str">
+        <v>PASS</v>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
+        <v>Filled: Nationality</v>
+      </c>
+      <c r="O16" t="str">
+        <v>screenshots/STEP_15.png</v>
+      </c>
+      <c r="P16" t="str">
+        <v>page_sources/STEP_15_source.html</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -902,6 +1007,21 @@
       </c>
       <c r="K17" t="str">
         <v xml:space="preserve">Gender should clicked </v>
+      </c>
+      <c r="L17" t="str">
+        <v>FAIL</v>
+      </c>
+      <c r="M17" t="str">
+        <v>Could not click element</v>
+      </c>
+      <c r="N17" t="str">
+        <v>Failed to click: Gender</v>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
Update: Test results, screenshots, and spreadsheet data
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -487,24 +487,24 @@
         <v xml:space="preserve">URL is opened </v>
       </c>
       <c r="L2" t="str">
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="M2" t="str">
+        <v>Cannot read properties of null (reading 'isClosed')</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Cannot read properties of null (reading 'isClosed')</v>
+      </c>
+      <c r="O2" t="str">
         <v/>
       </c>
-      <c r="N2" t="str">
-        <v>Opened: https://10.0.49.147:7504/FCJNeoWeb/SMMDIFRM.jsp</v>
-      </c>
-      <c r="O2" t="str">
-        <v>screenshots/STEP_1.png</v>
-      </c>
       <c r="P2" t="str">
-        <v>page_sources/STEP_1_source.html</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F3" t="str">
         <v>TS001TC001TSP002</v>
@@ -524,25 +524,10 @@
       <c r="K3" t="str">
         <v>username should be entered</v>
       </c>
-      <c r="L3" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M3" t="str">
-        <v/>
-      </c>
-      <c r="N3" t="str">
-        <v>Filled: USER ID</v>
-      </c>
-      <c r="O3" t="str">
-        <v>screenshots/STEP_2.png</v>
-      </c>
-      <c r="P3" t="str">
-        <v>page_sources/STEP_2_source.html</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F4" t="str">
         <v>TS001TC001TSP003</v>
@@ -562,25 +547,10 @@
       <c r="K4" t="str">
         <v>password should be entered</v>
       </c>
-      <c r="L4" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
-        <v>Filled: Password</v>
-      </c>
-      <c r="O4" t="str">
-        <v>screenshots/STEP_3.png</v>
-      </c>
-      <c r="P4" t="str">
-        <v>page_sources/STEP_3_source.html</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F5" t="str">
         <v>TS001TC001TSP004</v>
@@ -600,7 +570,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F6" t="str">
         <v>TS001TC001TSP005</v>
@@ -672,7 +642,7 @@
         <v>TS001TC002TSP003</v>
       </c>
       <c r="G9" t="str">
-        <v xml:space="preserve">Click Enter Query </v>
+        <v>Click New</v>
       </c>
       <c r="H9" t="str">
         <v>click</v>
@@ -1217,7 +1187,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="B34" t="str">
         <v>TS002</v>
@@ -1249,7 +1219,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F35" t="str">
         <v>TS111TC001TSP002</v>
@@ -1269,7 +1239,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F36" t="str">
         <v>TS111TC001TSP003</v>
@@ -1289,7 +1259,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F37" t="str">
         <v>TS111TC001TSP004</v>
@@ -1309,7 +1279,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F38" t="str">
         <v>TS111TC001TSP005</v>
@@ -1329,7 +1299,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F39" t="str">
         <v>TS111TC001TSP006</v>
@@ -1349,7 +1319,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>YES</v>
+        <v>NO</v>
       </c>
       <c r="F40" t="str">
         <v>TS111TC001TSP007</v>

</xml_diff>

<commit_message>
ENHANCED OVERLAY DETECTION: Aggressive scanning for ANY overlay/dialog + direct JavaScript element walking within containers - Now finds Customer Maintenance and custom Oracle dialogs
</commit_message>
<xml_diff>
--- a/RESULTS/Test_Results.xlsx
+++ b/RESULTS/Test_Results.xlsx
@@ -638,19 +638,19 @@
         <v>Fucntion Id should be filled with STDCIF</v>
       </c>
       <c r="L7" t="str">
-        <v>PASS</v>
+        <v>FAIL</v>
       </c>
       <c r="M7" t="str">
+        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
+      </c>
+      <c r="N7" t="str">
+        <v>page.waitForTimeout: Target page, context or browser has been closed</v>
+      </c>
+      <c r="O7" t="str">
         <v/>
       </c>
-      <c r="N7" t="str">
-        <v>Filled: Function Id</v>
-      </c>
-      <c r="O7" t="str">
-        <v>screenshots/STEP_6.png</v>
-      </c>
       <c r="P7" t="str">
-        <v>page_sources/STEP_6_source.html</v>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -672,21 +672,6 @@
       <c r="K8" t="str">
         <v xml:space="preserve">GO button should be clicked </v>
       </c>
-      <c r="L8" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
-        <v>Clicked: Go</v>
-      </c>
-      <c r="O8" t="str">
-        <v>screenshots/STEP_7.png</v>
-      </c>
-      <c r="P8" t="str">
-        <v>page_sources/STEP_7_source.html</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -707,21 +692,6 @@
       <c r="K9" t="str">
         <v xml:space="preserve">New should be clicked </v>
       </c>
-      <c r="L9" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M9" t="str">
-        <v/>
-      </c>
-      <c r="N9" t="str">
-        <v>Clicked: New</v>
-      </c>
-      <c r="O9" t="str">
-        <v>screenshots/STEP_8.png</v>
-      </c>
-      <c r="P9" t="str">
-        <v>page_sources/STEP_8_source.html</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -742,21 +712,6 @@
       <c r="K10" t="str">
         <v>P should be clicked and Customer No should be generated</v>
       </c>
-      <c r="L10" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M10" t="str">
-        <v/>
-      </c>
-      <c r="N10" t="str">
-        <v>Clicked: P</v>
-      </c>
-      <c r="O10" t="str">
-        <v>screenshots/STEP_9.png</v>
-      </c>
-      <c r="P10" t="str">
-        <v>page_sources/STEP_9_source.html</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -780,21 +735,6 @@
       <c r="K11" t="str">
         <v xml:space="preserve">First name should be filled </v>
       </c>
-      <c r="L11" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M11" t="str">
-        <v/>
-      </c>
-      <c r="N11" t="str">
-        <v>Filled: Full Name</v>
-      </c>
-      <c r="O11" t="str">
-        <v>screenshots/STEP_10.png</v>
-      </c>
-      <c r="P11" t="str">
-        <v>page_sources/STEP_10_source.html</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -818,21 +758,6 @@
       <c r="K12" t="str">
         <v xml:space="preserve">Short namae should be filled </v>
       </c>
-      <c r="L12" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M12" t="str">
-        <v/>
-      </c>
-      <c r="N12" t="str">
-        <v>Filled: Short Name</v>
-      </c>
-      <c r="O12" t="str">
-        <v>screenshots/STEP_11.png</v>
-      </c>
-      <c r="P12" t="str">
-        <v>page_sources/STEP_11_source.html</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -855,21 +780,6 @@
       </c>
       <c r="K13" t="str">
         <v>Customer category  should be filled</v>
-      </c>
-      <c r="L13" t="str">
-        <v>PASS</v>
-      </c>
-      <c r="M13" t="str">
-        <v/>
-      </c>
-      <c r="N13" t="str">
-        <v>Filled: Customer Category</v>
-      </c>
-      <c r="O13" t="str">
-        <v>screenshots/STEP_12.png</v>
-      </c>
-      <c r="P13" t="str">
-        <v>page_sources/STEP_12_source.html</v>
       </c>
     </row>
     <row r="14">

</xml_diff>